<commit_message>
commit all  changes of the second project
</commit_message>
<xml_diff>
--- a/sleniumTestNGDemo/excel/data.xlsx
+++ b/sleniumTestNGDemo/excel/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="registerInfo" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="75">
   <si>
     <t>email</t>
   </si>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,6 +802,9 @@
       <c r="O2" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="P2" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -849,6 +852,9 @@
       <c r="O3" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="P3" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -896,6 +902,9 @@
       <c r="O4" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="P4" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -943,6 +952,9 @@
       <c r="O5" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="P5" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -990,6 +1002,9 @@
       <c r="O6" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="P6" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1036,6 +1051,9 @@
       </c>
       <c r="O7" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1488,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>